<commit_message>
VAS , KEY account changes
</commit_message>
<xml_diff>
--- a/asn_lessThan100Cases.xlsx
+++ b/asn_lessThan100Cases.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="lessThan100Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="volBands" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -37,10 +38,10 @@
     <t>dStyles</t>
   </si>
   <si>
-    <t>acBandsPalletsSum</t>
-  </si>
-  <si>
-    <t>dBandCasesSum</t>
+    <t>abBandsPalletsSum</t>
+  </si>
+  <si>
+    <t>cdBandCasesSum</t>
   </si>
   <si>
     <t>20200118</t>
@@ -173,6 +174,30 @@
   </si>
   <si>
     <t>20200831</t>
+  </si>
+  <si>
+    <t>volBand</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>skus</t>
+  </si>
+  <si>
+    <t>shipments</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -372,10 +397,10 @@
         <v>3</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -468,10 +493,10 @@
         <v>3</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -628,10 +653,10 @@
         <v>22</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -660,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -788,10 +813,10 @@
         <v>5</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>15</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -980,10 +1005,10 @@
         <v>9</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1012,10 +1037,10 @@
         <v>3</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1044,10 +1069,10 @@
         <v>7</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>154</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1076,10 +1101,10 @@
         <v>2</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1108,10 +1133,10 @@
         <v>32</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>39</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1140,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1268,10 +1293,10 @@
         <v>1</v>
       </c>
       <c r="I33" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1524,10 +1549,10 @@
         <v>2</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>53</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1588,10 +1613,10 @@
         <v>1</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1656,6 +1681,149 @@
       </c>
       <c r="J45" s="0" t="n">
         <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1362</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1335269</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>215304</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>9665</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>8972.03</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>921</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2657</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>721043</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>105543</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5944</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4399.5</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>2119</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3116</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>376102</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>52903</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3116</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2206.11</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2719</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>8445</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>283116</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>39133</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>8444</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1634.35</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>6871</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>